<commit_message>
Falta apenas o Report
</commit_message>
<xml_diff>
--- a/src/main/resources/TDD_AdvantageOnlineShoppingData.xlsx
+++ b/src/main/resources/TDD_AdvantageOnlineShoppingData.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george.junior\eclipse-XPTO\TDD_AdvantageOnlineShopping\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCC3060-0A01-43C4-9FC9-6D2DA93CAE89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04FFF27-3FD6-4556-BEF7-9DD8BF1F0C5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-30" windowWidth="20640" windowHeight="11160" tabRatio="586" activeTab="1" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
+    <workbookView xWindow="-20610" yWindow="2070" windowWidth="20730" windowHeight="11160" tabRatio="586" firstSheet="3" activeTab="3" xr2:uid="{D4DEB64E-DE7E-45FC-8D49-61962D919F60}"/>
   </bookViews>
   <sheets>
-    <sheet name="AcessarUmProdutoPelaHome_P" sheetId="1" r:id="rId1"/>
-    <sheet name="AcessarUmProdutoPelaHome_N" sheetId="7" r:id="rId2"/>
-    <sheet name="CadastrarNovoCliente_P" sheetId="3" r:id="rId3"/>
-    <sheet name="CadastrarNovoCliente_N" sheetId="4" r:id="rId4"/>
-    <sheet name="BuscarUmProdutoPelaBusca_P" sheetId="5" r:id="rId5"/>
-    <sheet name="BuscarUmProdutoPelaBusca_N" sheetId="6" r:id="rId6"/>
+    <sheet name="AcessarUmProdutoPelaHome_Po" sheetId="1" r:id="rId1"/>
+    <sheet name="AcessarUmProdutoPelaHome_Ne" sheetId="7" r:id="rId2"/>
+    <sheet name="CadastrarNovoCliente_Po" sheetId="3" r:id="rId3"/>
+    <sheet name="CadastrarNovoCliente_Ne" sheetId="4" r:id="rId4"/>
+    <sheet name="BuscarUmProdutoPelaBusca_Po" sheetId="5" r:id="rId5"/>
+    <sheet name="BuscarUmProdutoPelaBusca_Ne" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,24 +38,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
   <si>
-    <t>idCategoria</t>
-  </si>
-  <si>
     <t>produto</t>
   </si>
   <si>
-    <t>headphonesTxt</t>
-  </si>
-  <si>
-    <t>laptopsTxt</t>
-  </si>
-  <si>
     <t>HP Stream - 11-d020nr Laptop</t>
   </si>
   <si>
-    <t>deveAbrirPaginaDeUmProdutoPelaCategoriaComSucesso</t>
-  </si>
-  <si>
     <t>DeveRealisarUmaBuscaComSucesso</t>
   </si>
   <si>
@@ -65,9 +53,6 @@
     <t>BOSE SOUNDLINK AROUND-EAR WIRELESS HEADPHONES II</t>
   </si>
   <si>
-    <t>DeveRealisarUmaBuscaComFalha</t>
-  </si>
-  <si>
     <t>Iphone</t>
   </si>
   <si>
@@ -77,9 +62,6 @@
     <t>Xiaomi</t>
   </si>
   <si>
-    <t>DeveCadasTrarUmNovoClienteComSucesso</t>
-  </si>
-  <si>
     <t>nomeusuario</t>
   </si>
   <si>
@@ -158,18 +140,6 @@
     <t>HP H2310 In-ear Headset</t>
   </si>
   <si>
-    <t>deveAbrirPaginaDeUmProdutoPelaCategoriaComFalha</t>
-  </si>
-  <si>
-    <t>speakersTxt</t>
-  </si>
-  <si>
-    <t>tabletsTxt</t>
-  </si>
-  <si>
-    <t>miceTxt</t>
-  </si>
-  <si>
     <t>HP Roar Wireless Speaker</t>
   </si>
   <si>
@@ -183,6 +153,36 @@
   </si>
   <si>
     <t>Ipad</t>
+  </si>
+  <si>
+    <t>SPEAKERS</t>
+  </si>
+  <si>
+    <t>TABLETS</t>
+  </si>
+  <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t>LAPTOPS</t>
+  </si>
+  <si>
+    <t>MICE</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>deveTentarAbrirPaginaDeUmProdutoInesistentePelaCategoria</t>
+  </si>
+  <si>
+    <t>deveAbrirPaginaDeUmProdutoPelaCategoria</t>
+  </si>
+  <si>
+    <t>DeveRealisarUmaBuscaDeProdutoInvalido</t>
+  </si>
+  <si>
+    <t>DeveTentarCadasTrarUmNovoClienteComFalha</t>
   </si>
 </sst>
 </file>
@@ -557,9 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80702A83-724E-4768-B1BE-90F73797AA16}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B2:B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -570,45 +568,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +614,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -629,9 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B404657F-C05F-2A44-AAD2-7863EF0C7397}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -642,45 +638,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -688,7 +684,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -700,9 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47748592-BB78-41A0-8ED8-959B95E0445B}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="A1:M4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -718,78 +712,78 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H2">
         <v>989997979</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <v>18060605</v>
@@ -797,37 +791,37 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H3">
         <v>989997979</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M3">
         <v>18060605</v>
@@ -835,37 +829,37 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>989997979</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M4">
         <v>18060605</v>
@@ -885,13 +879,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A2C4E6-CCD4-41FE-AB5C-3F2F51B1DE80}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
@@ -905,78 +899,78 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H2">
         <v>989997979</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M2">
         <v>18060605</v>
@@ -984,34 +978,34 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H3">
         <v>989997979</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M3">
         <v>18060605</v>
@@ -1019,37 +1013,37 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H4">
         <v>989997979</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="M4">
         <v>18060605</v>
@@ -1069,9 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC3573-0780-4934-A8A2-22FE942CCBF3}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1081,25 +1073,25 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1112,36 +1104,36 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>